<commit_message>
[feat] 修改导入模版 related to issue #1
</commit_message>
<xml_diff>
--- a/src/assets/files/商机导入模板.xlsx
+++ b/src/assets/files/商机导入模板.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11015"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10512"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kelly/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kelly/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67DCAB68-546A-1341-997B-76551E0746DA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BC23164-7C54-3541-A967-3EEAEF8FEDCD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <r>
       <rPr>
@@ -74,19 +74,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">02163561133	</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">02152534888	</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">15800698198	</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">02164647155	</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -155,276 +143,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>上海影响力企业管理咨询有限公司</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>易发梨</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>杨亮</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>金山区市场监管局</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>上海同济科技园孵化器有限公司</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>浦东新区市场监管局</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>上海恺润思投资管理有限公司</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>夏天勃</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>法人张磊</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>注册时间</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>2018-01-01</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>上海敏众投资管理有限公司</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>蒋仲德</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>上海海湾科技园发展有限公司</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>陈兰</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>上海耀华教育管理有限公司</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>叶允鸿</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>上海聚阳投资管理有限公司</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>钱俊杰</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>上海禧溢投资管理有限公司</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>上海融财商务咨询有限公司</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>沈步英</t>
-    </r>
-  </si>
-  <si>
     <t>公司名称（必填）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -469,7 +187,6 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Microsoft YaHei UI"/>
-        <charset val="134"/>
       </rPr>
       <t>1</t>
     </r>
@@ -489,7 +206,6 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Microsoft YaHei UI"/>
-        <charset val="134"/>
       </rPr>
       <t>2</t>
     </r>
@@ -523,14 +239,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>13321821217;02158810914</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">02133658380;02133655722	</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>复制粘贴到模版时,最好选择数值粘贴(不带格式的粘贴)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -548,6 +256,14 @@
   </si>
   <si>
     <t>一次性导入数量,尽量不超过5千,否则会影响上传速度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>注册时间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-01-01</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -596,12 +312,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Microsoft YaHei UI"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <sz val="14"/>
       <color theme="1"/>
       <name val="SimSun"/>
@@ -614,6 +324,11 @@
       <name val="SimSun"/>
       <family val="3"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Microsoft YaHei UI"/>
     </font>
   </fonts>
   <fills count="4">
@@ -663,12 +378,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="176" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -683,7 +398,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -692,19 +407,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="177" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -716,8 +431,11 @@
     <xf numFmtId="177" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1057,10 +775,10 @@
   <sheetPr>
     <tabColor theme="8"/>
   </sheetPr>
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="26" customHeight="1"/>
@@ -1072,19 +790,20 @@
     <col min="5" max="5" width="25.6640625" style="16" customWidth="1"/>
     <col min="6" max="6" width="18.1640625" style="4" customWidth="1"/>
     <col min="7" max="7" width="25.6640625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="52.6640625" style="4" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="4"/>
+    <col min="8" max="8" width="25.6640625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="52.6640625" style="4" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="6" customFormat="1" ht="36" customHeight="1">
+    <row r="1" spans="1:9" s="6" customFormat="1" ht="36" customHeight="1">
       <c r="A1" s="5" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
@@ -1093,27 +812,30 @@
         <v>1</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="26" customHeight="1">
+    <row r="2" spans="1:9" ht="26" customHeight="1">
       <c r="A2" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E2" s="16">
         <v>63561133828</v>
@@ -1122,214 +844,13 @@
         <v>1</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="26" customHeight="1">
-      <c r="A3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="16">
-        <v>2164647155</v>
-      </c>
-      <c r="F3" s="4">
-        <v>1</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="26" customHeight="1">
-      <c r="A4" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="16">
-        <v>2164647156</v>
-      </c>
-      <c r="F4" s="4">
-        <v>2</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="26" customHeight="1">
-      <c r="A5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="16">
-        <v>2164647157</v>
-      </c>
-      <c r="F5" s="4">
-        <v>1</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="26" customHeight="1">
-      <c r="A6" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="16">
-        <v>12180235566</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="16">
-        <v>2164647158</v>
-      </c>
-      <c r="F6" s="4">
-        <v>1</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="26" customHeight="1">
-      <c r="A7" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="16">
-        <v>2151753633</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="16">
-        <v>2164647159</v>
-      </c>
-      <c r="F7" s="4">
-        <v>2</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="26" customHeight="1">
-      <c r="A8" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="16">
-        <v>13901957098</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="16">
-        <v>2164647160</v>
-      </c>
-      <c r="F8" s="4">
-        <v>1</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="26" customHeight="1">
-      <c r="A9" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="16">
-        <v>2164647161</v>
-      </c>
-      <c r="F9" s="4">
-        <v>1</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="26" customHeight="1">
-      <c r="A10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="16">
-        <v>2164647162</v>
-      </c>
-      <c r="F10" s="4">
-        <v>1</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="26" customHeight="1">
-      <c r="A11" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="16">
-        <v>13801902604</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="16">
-        <v>2164647163</v>
+      <c r="I2" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1345,8 +866,8 @@
   </sheetPr>
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="33.1640625" defaultRowHeight="26" customHeight="1"/>
@@ -1359,20 +880,20 @@
   <sheetData>
     <row r="1" spans="1:5" ht="37" customHeight="1">
       <c r="A1" s="18" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="B1" s="18"/>
       <c r="C1" s="18"/>
     </row>
     <row r="2" spans="1:5" ht="26" customHeight="1">
       <c r="A2" s="7" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="9"/>
@@ -1382,10 +903,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="9"/>
@@ -1395,10 +916,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>43</v>
+        <v>20</v>
       </c>
       <c r="D4" s="8"/>
       <c r="E4" s="9"/>
@@ -1408,10 +929,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="9"/>
@@ -1421,10 +942,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="9"/>
@@ -1434,10 +955,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="9"/>
@@ -1447,10 +968,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="D8" s="8"/>
       <c r="E8" s="9"/>

</xml_diff>